<commit_message>
added pv and seasonal variants
</commit_message>
<xml_diff>
--- a/output/res_trafo/loading_percent.xlsx
+++ b/output/res_trafo/loading_percent.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>87.05903679059473</v>
+        <v>48.75323856031761</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>80.59518498549288</v>
+        <v>48.10036469736591</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>79.93322954709384</v>
+        <v>47.85010208201233</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>79.37268953271152</v>
+        <v>47.17832111586508</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>78.78034897712205</v>
+        <v>46.40877999284862</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>79.30607991188975</v>
+        <v>45.36340335784689</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>78.37972667803328</v>
+        <v>44.10713217741337</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>72.55546531543226</v>
+        <v>35.38532249257068</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>65.03738376767363</v>
+        <v>20.63278040443107</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>62.83995664660505</v>
+        <v>8.556497084989612</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>62.66150385173804</v>
+        <v>14.3183330111775</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>66.028476122188</v>
+        <v>23.35464860662984</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>69.98082527532532</v>
+        <v>28.66350259985149</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>72.05353769568235</v>
+        <v>21.52029925950538</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>73.4399416486996</v>
+        <v>18.63703151586877</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>77.26987446614754</v>
+        <v>19.17210934423268</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>85.53628568313928</v>
+        <v>18.28448011559187</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>94.50934658007606</v>
+        <v>28.2273126580121</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>101.4461370798005</v>
+        <v>40.08645810907587</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>105.5621089072078</v>
+        <v>50.93024410622174</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>107.6451848728956</v>
+        <v>58.98491584267725</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>105.5794383598936</v>
+        <v>59.67913773675354</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>102.2374443038729</v>
+        <v>56.9065969243132</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>96.52109215833428</v>
+        <v>53.27662212033255</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>89.55763210745235</v>
+        <v>51.55309065714001</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>83.41757525420368</v>
+        <v>51.00218454763724</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>82.78582925284343</v>
+        <v>53.22452957468968</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>80.91194152248843</v>
+        <v>50.48721754163776</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>81.29097477087778</v>
+        <v>50.17503506452424</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>79.85686451478414</v>
+        <v>49.4239132788661</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>79.5272464196207</v>
+        <v>46.85984391776666</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>75.52296073345678</v>
+        <v>36.33005626702732</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>70.22490910528177</v>
+        <v>12.62320858927185</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>65.12488764343649</v>
+        <v>12.70003107400009</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>63.0760457095386</v>
+        <v>31.46182554354613</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>65.41307234355973</v>
+        <v>34.93566759323897</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>68.83680403731701</v>
+        <v>30.42903449397697</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>70.87959089522552</v>
+        <v>29.65676101778318</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>73.52619286851061</v>
+        <v>21.11915236526646</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>78.43846561339863</v>
+        <v>15.56989279932784</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>86.80106800404641</v>
+        <v>18.82563086470025</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>95.03338958672084</v>
+        <v>23.32960291582058</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>99.21184910556403</v>
+        <v>34.82605710064902</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>102.7550550871904</v>
+        <v>46.62568298681386</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>104.5675565226528</v>
+        <v>56.60655943147247</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>103.9242689058284</v>
+        <v>59.71978794030621</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>100.1588859955061</v>
+        <v>57.70367072842533</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>95.12554540724433</v>
+        <v>52.7347855887479</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>87.4033379746021</v>
+        <v>51.33057455883458</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>83.25411368754146</v>
+        <v>50.86124096590141</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>81.78256246145303</v>
+        <v>50.68112637898948</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>80.43813329711334</v>
+        <v>51.24805083929927</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>78.7839294780461</v>
+        <v>50.14175689166274</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>77.7597915406608</v>
+        <v>49.76633987126651</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>78.49586462724847</v>
+        <v>47.17841935496615</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>77.41729893710095</v>
+        <v>38.29510828723976</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>74.83633886287758</v>
+        <v>19.71455877334926</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>69.91200256176691</v>
+        <v>6.732877596740555</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>67.27772711339642</v>
+        <v>24.52975027638288</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>67.36099083093873</v>
+        <v>37.24717906535607</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>69.97136911924042</v>
+        <v>39.23539890684511</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>72.08307611015931</v>
+        <v>36.45854748515903</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>74.95275837604967</v>
+        <v>30.35194481872264</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>79.30438715387257</v>
+        <v>21.87679897796867</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>86.45689194666851</v>
+        <v>13.15134282784816</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>93.13728051242472</v>
+        <v>15.92983940304014</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>97.91147332131153</v>
+        <v>29.75372955494493</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>101.3573511455914</v>
+        <v>45.65540732677202</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>101.8814456435671</v>
+        <v>55.06142437830223</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>101.076523969669</v>
+        <v>57.36969879279476</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>97.94312992865525</v>
+        <v>55.21351863641474</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>92.70781281863422</v>
+        <v>50.70954595045995</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>87.00429121183275</v>
+        <v>48.95699971498605</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>82.67487112292245</v>
+        <v>48.17632542362561</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>81.6161947889498</v>
+        <v>48.25483460130832</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>81.17001869077527</v>
+        <v>49.08787907715023</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>79.16004793953721</v>
+        <v>48.41506033755302</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>77.99440629575855</v>
+        <v>47.45030862797974</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>77.70303677761355</v>
+        <v>44.95043914330191</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>77.0268069801465</v>
+        <v>36.07270461467449</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>73.02829171736775</v>
+        <v>20.2470566056404</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>67.14488274153115</v>
+        <v>7.342445598489309</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>64.84484445842192</v>
+        <v>16.07678998820193</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>65.23005437474272</v>
+        <v>25.28748829332434</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>66.95944335860393</v>
+        <v>33.1948449647924</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>69.26189994705646</v>
+        <v>32.26946084694153</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>72.11366521157089</v>
+        <v>27.77246221560314</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>75.76510533059395</v>
+        <v>24.41133637467258</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>83.13984766354474</v>
+        <v>11.65432090499096</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>90.5125063871801</v>
+        <v>11.89141650688275</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>96.46458149335344</v>
+        <v>27.52995744253111</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>100.3236921522594</v>
+        <v>40.35873239942786</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>102.546291672626</v>
+        <v>50.27462094602414</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>102.5991651803783</v>
+        <v>53.9406246390166</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>99.42390658564466</v>
+        <v>52.14606507162897</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>93.61536276395725</v>
+        <v>48.68889045177264</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>87.6668536545057</v>
+        <v>47.40669785368222</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>82.9277052918671</v>
+        <v>46.43281383905503</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>80.6624884668512</v>
+        <v>45.90874914139093</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>80.80178407678122</v>
+        <v>44.9389152797046</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>79.81414251325371</v>
+        <v>46.01625503613561</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>78.30750066442207</v>
+        <v>45.57924260652769</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>77.37127502832527</v>
+        <v>44.42022476379551</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>74.86032261957398</v>
+        <v>37.57363879349214</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>69.71001451149401</v>
+        <v>21.81542410827414</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>64.56044099237168</v>
+        <v>4.037003619641491</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>64.03465725944942</v>
+        <v>13.15960928872346</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>65.38612838276433</v>
+        <v>20.55513857753125</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>67.72022989681459</v>
+        <v>19.56056367938244</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>70.43403106423504</v>
+        <v>18.396510279572</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>74.11117283502925</v>
+        <v>20.55033871593381</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>77.4274463150263</v>
+        <v>21.91079918511869</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>84.76359006146103</v>
+        <v>10.15493684959367</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>90.2394616503785</v>
+        <v>12.36642388125862</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>95.94050070053279</v>
+        <v>26.98159651737944</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>97.81017202074096</v>
+        <v>43.5567143108369</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>100.6857635308723</v>
+        <v>49.13493691800913</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>101.3666828598466</v>
+        <v>52.03650529196228</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>99.19303188214185</v>
+        <v>51.01918893577083</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>93.56402584351311</v>
+        <v>48.9142420643792</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>91.75868033697132</v>
+        <v>50.55769661024607</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>86.70423470418356</v>
+        <v>49.77400088422254</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>85.54870648245257</v>
+        <v>49.50495653413675</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>84.9559857710093</v>
+        <v>48.60549057826405</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>84.71332202529489</v>
+        <v>48.12269098437234</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>83.68287946167565</v>
+        <v>47.51529586516391</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>83.59332200623658</v>
+        <v>46.77887349998218</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>80.67947801017652</v>
+        <v>37.26884228624392</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>77.76769532216341</v>
+        <v>20.71001531555411</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>73.25857848934932</v>
+        <v>7.80683073527926</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>73.08190418504668</v>
+        <v>28.02473706266695</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>76.0369476621062</v>
+        <v>37.14472282881547</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>77.44865215867775</v>
+        <v>31.86309639883952</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>79.85650474546077</v>
+        <v>27.1189842803541</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>82.47592331864173</v>
+        <v>22.85550083145351</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>86.59173521969345</v>
+        <v>18.56755098034724</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>93.92358490475957</v>
+        <v>9.573705328122497</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>100.3599088908659</v>
+        <v>13.62454237838885</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>106.7751518949637</v>
+        <v>31.46822989323714</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>110.8016174142283</v>
+        <v>44.77226099766938</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>112.0850043907418</v>
+        <v>51.23013007011237</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>110.7705040719451</v>
+        <v>53.89492130142661</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>106.3441236841101</v>
+        <v>53.04828684033842</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>99.61079148479367</v>
+        <v>51.05829963863697</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>92.37959482651948</v>
+        <v>51.12974235523138</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>86.82206566599938</v>
+        <v>50.79267466799517</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>86.38050619445146</v>
+        <v>50.31478613809266</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>84.19995221167268</v>
+        <v>48.92393455559663</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>84.43215116873381</v>
+        <v>47.17770944429204</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>84.03714985967731</v>
+        <v>46.41337774943752</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>83.30108755807004</v>
+        <v>44.63029378177906</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>80.48180047543786</v>
+        <v>36.52381526605617</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>76.07126732027334</v>
+        <v>16.84127304879738</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>71.25081770867581</v>
+        <v>6.770104995597534</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>73.56832535217214</v>
+        <v>21.83054918346592</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>76.27951923528417</v>
+        <v>34.2104207120366</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>79.0950064534469</v>
+        <v>36.78487103576281</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>80.97738301571508</v>
+        <v>31.73638398777054</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>83.42899261330739</v>
+        <v>21.84069615159085</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>87.65354097833728</v>
+        <v>17.35411353268182</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>95.75076906399696</v>
+        <v>10.95680230296947</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>102.4019622249168</v>
+        <v>23.72368078597645</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>106.7680375758373</v>
+        <v>36.67571873249413</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>109.7151497808372</v>
+        <v>47.86062374686173</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>111.155344192043</v>
+        <v>56.5063933309627</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>109.614866759695</v>
+        <v>57.99421313488281</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>104.8160628092636</v>
+        <v>55.89866851943762</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>98.5554606698004</v>
+        <v>52.1436723089468</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
opf works with voltage only
</commit_message>
<xml_diff>
--- a/output/res_trafo/loading_percent.xlsx
+++ b/output/res_trafo/loading_percent.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>53.79405852065703</v>
+        <v>38.5336236235199</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>53.18912551308583</v>
+        <v>35.27129997163557</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>52.92778606773363</v>
+        <v>35.09245743556239</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>52.21448677662306</v>
+        <v>35.92756251036415</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>51.31309967839584</v>
+        <v>37.130156996377</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>50.08750613898813</v>
+        <v>39.00275762081579</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>49.26595025758285</v>
+        <v>42.192985584269</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>44.19611235345962</v>
+        <v>47.91508570951046</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>38.44448237350854</v>
+        <v>50.34095230988</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>38.40138839921075</v>
+        <v>44.25647948902807</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>41.11332503555604</v>
+        <v>26.35833740473258</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>43.35767254328874</v>
+        <v>27.37542248294274</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>43.40741251761504</v>
+        <v>29.5815199755564</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>42.60018236208481</v>
+        <v>27.91619368663332</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>42.47296580285492</v>
+        <v>30.79426692016003</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>44.66728302034861</v>
+        <v>42.61688650998624</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>48.27394573580877</v>
+        <v>62.76487806631222</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>52.01440697184424</v>
+        <v>70.53707797549879</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>56.50241129874247</v>
+        <v>73.30317892321477</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>60.74033663635654</v>
+        <v>71.37656055492961</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>65.25997770118627</v>
+        <v>65.90553464997818</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>65.53629283611878</v>
+        <v>58.54885792946276</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>62.73685535758285</v>
+        <v>51.87634649751196</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>58.89792802341528</v>
+        <v>45.10129232176062</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>57.036009010938</v>
+        <v>40.3366216521827</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>56.45923353384133</v>
+        <v>37.47215831754374</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>59.15745980362331</v>
+        <v>38.05437939236548</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>56.05330060183078</v>
+        <v>37.95493224109528</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>55.67479764552908</v>
+        <v>39.44394029001089</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>54.64445779866787</v>
+        <v>42.03054019801191</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>52.76525739791761</v>
+        <v>44.87380583801979</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>47.14376861759833</v>
+        <v>48.65757590410652</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>36.66285269041403</v>
+        <v>50.2497245922264</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>35.58596508621341</v>
+        <v>35.69387227664009</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>40.56630582191556</v>
+        <v>12.81109506423192</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>42.68715229294997</v>
+        <v>12.10339429018721</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>42.26664857937738</v>
+        <v>13.42189125067878</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>41.44302047642412</v>
+        <v>15.28640975215582</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>42.45281011198879</v>
+        <v>24.2498292839352</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>45.52444140066539</v>
+        <v>42.88635612864446</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>47.64150126993009</v>
+        <v>62.53059101488257</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>49.57416996676159</v>
+        <v>71.49588906702839</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>54.18415135994483</v>
+        <v>72.79935304917014</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>59.01918480480652</v>
+        <v>71.24502750512464</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>62.95624453209258</v>
+        <v>65.95570926953171</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>65.64248341885343</v>
+        <v>59.13397869726411</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>63.56478409969818</v>
+        <v>51.91384637540671</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>58.1871923884413</v>
+        <v>45.34537969208408</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>56.71452226324457</v>
+        <v>39.90129143830648</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>56.3804498929553</v>
+        <v>37.3846885497515</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>56.15354203488378</v>
+        <v>37.06305595202222</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>56.84323773044754</v>
+        <v>37.56694856945531</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>55.52199352731648</v>
+        <v>38.66820476906013</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>55.08387296770822</v>
+        <v>41.34289408040923</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>53.0154704015435</v>
+        <v>45.37243547895283</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>48.91970110542355</v>
+        <v>48.77635075757679</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>40.03229497278977</v>
+        <v>50.88362530930449</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>36.02777707727917</v>
+        <v>36.82915983014885</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>38.93582138414327</v>
+        <v>16.16963662985445</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>43.03767617724942</v>
+        <v>4.543117647150242</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>43.29020124497888</v>
+        <v>7.15296742427704</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>41.51874251674433</v>
+        <v>15.99915819544638</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>39.88557208999616</v>
+        <v>27.73794637604707</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>40.76325412733694</v>
+        <v>46.99818555487492</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>43.05247709594026</v>
+        <v>64.65796935127332</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>46.02482455526943</v>
+        <v>70.76630786233036</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>50.21289090641453</v>
+        <v>72.93601719593674</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>56.10601849604811</v>
+        <v>71.51620319703501</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>60.77455197052073</v>
+        <v>66.17769580561257</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>62.649278509056</v>
+        <v>57.90994882059871</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>60.69287709159986</v>
+        <v>50.49008238602404</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>55.74260864562444</v>
+        <v>44.18460739172085</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>54.0564252248367</v>
+        <v>39.02725949777118</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>53.2298520426078</v>
+        <v>36.31080968260656</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>53.42033679807665</v>
+        <v>35.62830227087378</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>54.40211176926864</v>
+        <v>36.47632600399345</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>53.69663626721876</v>
+        <v>37.88887137834444</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>52.42325674264933</v>
+        <v>40.78856813817734</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>50.2995604948413</v>
+        <v>44.49394816542497</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>46.87411743669321</v>
+        <v>47.78454168713542</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>40.41072186398099</v>
+        <v>48.97177480431002</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>37.21302712033729</v>
+        <v>33.96827823572238</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>38.03751171611049</v>
+        <v>16.59133383127459</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>39.847159259952</v>
+        <v>7.841733148483453</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>41.16693531640104</v>
+        <v>5.716468341419956</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>40.61528610023809</v>
+        <v>13.27602221148377</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>40.08902695772581</v>
+        <v>27.34424952152141</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>40.78657986629015</v>
+        <v>44.26592005988216</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>42.58316816125534</v>
+        <v>61.59261321021721</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>44.7613342388806</v>
+        <v>69.26935554130715</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>47.59459809583927</v>
+        <v>71.63469071471302</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>50.79949682932077</v>
+        <v>70.45934893962509</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>55.48326106534708</v>
+        <v>65.09768496945836</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>58.6986647005863</v>
+        <v>57.60983971017865</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>56.90209119609022</v>
+        <v>50.50608449748511</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>53.32894596270465</v>
+        <v>44.23668170039051</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>52.1217216364313</v>
+        <v>38.48874020379947</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>51.12233526615875</v>
+        <v>35.37679288652018</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>50.69311791075018</v>
+        <v>33.98878001875472</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>49.63578351289321</v>
+        <v>34.25891344516022</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>50.85441396708353</v>
+        <v>35.71794090767862</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>50.36832705376324</v>
+        <v>38.17097837310888</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>49.21538021689378</v>
+        <v>41.53842661896164</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>46.2823381872285</v>
+        <v>45.34064401782398</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>40.07539632778754</v>
+        <v>47.88245022741437</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>37.96668801158795</v>
+        <v>36.37925537102844</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>40.10927890143748</v>
+        <v>21.77378787457371</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>42.86033475892266</v>
+        <v>13.09786706264059</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>43.5435760857713</v>
+        <v>15.43492275024103</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>42.50662360256406</v>
+        <v>20.16029018412824</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>41.20740843731655</v>
+        <v>28.72847333237098</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>41.305928809047</v>
+        <v>45.10952861449835</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>43.46606178591143</v>
+        <v>63.11744264874743</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>45.35796615611088</v>
+        <v>69.19304128779982</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>47.24427920089585</v>
+        <v>71.44787831100084</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>52.29071974553379</v>
+        <v>66.60124982075556</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>53.53781152584774</v>
+        <v>61.10318645527121</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>56.61063396203725</v>
+        <v>54.93966700005691</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>55.73461520225849</v>
+        <v>49.82021250450344</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>53.59306500973469</v>
+        <v>43.69215732100776</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>55.68327263692393</v>
+        <v>40.54669231563441</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>55.01860939656456</v>
+        <v>36.32603656294081</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>54.87417516889163</v>
+        <v>35.24440750847005</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>53.88163774330184</v>
+        <v>35.05833221033428</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>53.29692546363568</v>
+        <v>36.37552644126544</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>52.5533849174103</v>
+        <v>37.91088946657828</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>52.05027596708156</v>
+        <v>41.09513507358876</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>47.66516677219864</v>
+        <v>46.75908007707611</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>42.06018394535329</v>
+        <v>52.71355137258262</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>40.38431512452512</v>
+        <v>49.75404360126679</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>46.38572119958621</v>
+        <v>38.91997766776474</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>50.6303477060103</v>
+        <v>36.62314935516316</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>49.63157457538097</v>
+        <v>33.75318898511347</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>47.27089984450385</v>
+        <v>41.1352651030347</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>44.9703908822782</v>
+        <v>46.78009461702231</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>43.56672864296674</v>
+        <v>57.33421688983811</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>45.33862772477069</v>
+        <v>70.86610547770044</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>47.80849176126407</v>
+        <v>75.98877233409968</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>51.68904521083443</v>
+        <v>76.92042216691284</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>53.92825037788636</v>
+        <v>73.38938438637366</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>55.93166462696201</v>
+        <v>66.38961151131851</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>58.53271358588186</v>
+        <v>59.9938005072943</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>58.06582494917814</v>
+        <v>53.31422539126781</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>56.05568158149833</v>
+        <v>46.56330397628213</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>56.41311698639289</v>
+        <v>40.78756687954799</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>56.28725197562962</v>
+        <v>37.27939337639029</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>55.88183961473221</v>
+        <v>36.19824571583222</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>54.22092964916519</v>
+        <v>35.74123304681906</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>52.24743500125503</v>
+        <v>36.74552785402163</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>51.24054341937071</v>
+        <v>38.44757792616835</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>49.33832310421775</v>
+        <v>41.51488896248188</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>46.36266961380183</v>
+        <v>47.78984023133718</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>40.67910036245495</v>
+        <v>52.61721286758997</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>41.44459957905074</v>
+        <v>48.276045728056</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>46.76783502177337</v>
+        <v>38.6968609990262</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>50.69266587398371</v>
+        <v>37.66993552806074</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>50.62646935975595</v>
+        <v>38.32864511562358</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>47.86035682260032</v>
+        <v>39.30261529165242</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>45.38717714522739</v>
+        <v>45.95661157591219</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>45.30831026420481</v>
+        <v>56.49468337611947</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>47.80437079148697</v>
+        <v>71.83328801157403</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>50.02323673760424</v>
+        <v>77.6193338452531</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>53.26318480380363</v>
+        <v>77.99333745467698</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>57.40692195555322</v>
+        <v>73.8475096209185</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>61.75802777874482</v>
+        <v>67.67544699872047</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>63.47637759365576</v>
+        <v>60.37560491101446</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>61.5373886081715</v>
+        <v>52.65385414974714</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>57.55223122290598</v>
+        <v>46.44888995790078</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
line loading is still broken
</commit_message>
<xml_diff>
--- a/output/res_trafo/loading_percent.xlsx
+++ b/output/res_trafo/loading_percent.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>38.5336236235199</v>
+        <v>26.92579227424842</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>35.27129997163557</v>
+        <v>25.57766581106461</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>35.09245743556239</v>
+        <v>25.16593926899765</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>35.92756251036415</v>
+        <v>25.08769358648623</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>37.130156996377</v>
+        <v>26.06202347904019</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>39.00275762081579</v>
+        <v>27.32257016277202</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>42.192985584269</v>
+        <v>27.49142968410301</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>47.91508570951046</v>
+        <v>17.37998780065877</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>50.34095230988</v>
+        <v>1.236022011315791</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>44.25647948902807</v>
+        <v>24.12471005124852</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>26.35833740473258</v>
+        <v>57.57009838134475</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>27.37542248294274</v>
+        <v>78.97677838347492</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>29.5815199755564</v>
+        <v>95.77363788451653</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>27.91619368663332</v>
+        <v>86.81603115398292</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>30.79426692016003</v>
+        <v>80.69877853283593</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>42.61688650998624</v>
+        <v>69.82881413012089</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>62.76487806631222</v>
+        <v>36.29756308424571</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>70.53707797549879</v>
+        <v>10.47275560225612</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>73.30317892321477</v>
+        <v>12.60242553151513</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>71.37656055492961</v>
+        <v>31.82128036228986</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>65.90553464997818</v>
+        <v>42.66206803933564</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>58.54885792946276</v>
+        <v>41.00772948882172</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>51.87634649751196</v>
+        <v>35.28528161767901</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>45.10129232176062</v>
+        <v>29.66245307552957</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>40.3366216521827</v>
+        <v>26.77922498039559</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>37.47215831754374</v>
+        <v>25.30707707403154</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>38.05437939236548</v>
+        <v>24.77608612305334</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>37.95493224109528</v>
+        <v>25.25038609881203</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>39.44394029001089</v>
+        <v>26.44301193374303</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>42.03054019801191</v>
+        <v>28.60253499832083</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>44.87380583801979</v>
+        <v>26.96919579045342</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>48.65757590410652</v>
+        <v>9.541160371321233</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>50.2497245922264</v>
+        <v>25.89130393529517</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>35.69387227664009</v>
+        <v>61.15194510776028</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>12.81109506423192</v>
+        <v>92.56853130144003</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>12.10339429018721</v>
+        <v>102.6474722192011</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>13.42189125067878</v>
+        <v>99.28445475770377</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>15.28640975215582</v>
+        <v>102.236904380467</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>24.2498292839352</v>
+        <v>83.8854236184623</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>42.88635612864446</v>
+        <v>53.28310686164581</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>62.53059101488257</v>
+        <v>35.64413576526199</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>71.49588906702839</v>
+        <v>22.83844145780652</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>72.79935304917014</v>
+        <v>1.689196285372581</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>71.24502750512464</v>
+        <v>23.21607688112587</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>65.95570926953171</v>
+        <v>40.76953993539522</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>59.13397869726411</v>
+        <v>41.0302989089926</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>51.91384637540671</v>
+        <v>35.45825453248555</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>45.34537969208408</v>
+        <v>29.75560903011817</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>39.90129143830648</v>
+        <v>27.26170555645828</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>37.3846885497515</v>
+        <v>25.84112676013008</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>37.06305595202222</v>
+        <v>25.31196405293171</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>37.56694856945531</v>
+        <v>25.21159247739277</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>38.66820476906013</v>
+        <v>26.76079420674157</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>41.34289408040923</v>
+        <v>28.44945880523121</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>45.37243547895283</v>
+        <v>27.24751313234805</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>48.77635075757679</v>
+        <v>10.43751239529088</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>50.88362530930449</v>
+        <v>19.07406138281398</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>36.82915983014885</v>
+        <v>51.32965956808364</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>16.16963662985445</v>
+        <v>81.90013608863961</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>4.543117647150242</v>
+        <v>104.0561577161946</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>7.15296742427704</v>
+        <v>110.8323138678788</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>15.99915819544638</v>
+        <v>110.696647897869</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>27.73794637604707</v>
+        <v>102.5255863049651</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>46.99818555487492</v>
+        <v>84.94380068669146</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>64.65796935127332</v>
+        <v>60.38803893362871</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>70.76630786233036</v>
+        <v>31.30562342955023</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>72.93601719593674</v>
+        <v>1.16312124797363</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>71.51620319703501</v>
+        <v>27.12841615607407</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>66.17769580561257</v>
+        <v>41.51114570893836</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>57.90994882059871</v>
+        <v>41.24755288500636</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>50.49008238602404</v>
+        <v>35.55274573232877</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>44.18460739172085</v>
+        <v>29.78801012943021</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>39.02725949777118</v>
+        <v>27.3679168945374</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>36.31080968260656</v>
+        <v>25.76982785624696</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>35.62830227087378</v>
+        <v>25.10514914123342</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>36.47632600399345</v>
+        <v>25.61133111922757</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>37.88887137834444</v>
+        <v>26.25843943985731</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>40.78856813817734</v>
+        <v>28.10781094993087</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>44.49394816542497</v>
+        <v>27.67846759713651</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>47.78454168713542</v>
+        <v>9.909360354011</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>48.97177480431002</v>
+        <v>17.20707375519618</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>33.96827823572238</v>
+        <v>46.20589670691698</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>16.59133383127459</v>
+        <v>71.57111683449516</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>7.841733148483453</v>
+        <v>88.38549069625159</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>5.716468341419956</v>
+        <v>104.363892307808</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>13.27602221148377</v>
+        <v>105.4216081066103</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>27.34424952152141</v>
+        <v>97.92656063942701</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>44.26592005988216</v>
+        <v>91.03472624904482</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>61.59261321021721</v>
+        <v>63.17017928223554</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>69.26935554130715</v>
+        <v>30.53579449121432</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>71.63469071471302</v>
+        <v>1.162344389698027</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>70.45934893962509</v>
+        <v>25.05917689228418</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>65.09768496945836</v>
+        <v>39.75823887770461</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>57.60983971017865</v>
+        <v>40.42700104299423</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>50.50608449748511</v>
+        <v>35.55232037620566</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>44.23668170039051</v>
+        <v>30.30903547101132</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>38.48874020379947</v>
+        <v>27.8957403615152</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>35.37679288652018</v>
+        <v>25.93901619353046</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>33.98878001875472</v>
+        <v>25.20610726689813</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>34.25891344516022</v>
+        <v>25.22906275067259</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>35.71794090767862</v>
+        <v>26.08295767535296</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>38.17097837310888</v>
+        <v>27.14265974023873</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>41.53842661896164</v>
+        <v>28.45766176144261</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>45.34064401782398</v>
+        <v>17.22880361330196</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>47.88245022741437</v>
+        <v>4.967412359346453</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>36.37925537102844</v>
+        <v>32.71954556731513</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>21.77378787457371</v>
+        <v>62.79661798453768</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>13.09786706264059</v>
+        <v>74.40700373377901</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>15.43492275024103</v>
+        <v>71.75788157028329</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>20.16029018412824</v>
+        <v>74.91537665355064</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>28.72847333237098</v>
+        <v>83.40806992843441</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>45.10952861449835</v>
+        <v>87.34717242106412</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>63.11744264874743</v>
+        <v>63.44797116062878</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>69.19304128779982</v>
+        <v>26.83689488601465</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>71.44787831100084</v>
+        <v>2.848200604200795</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>66.60124982075556</v>
+        <v>31.44909774182629</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>61.10318645527121</v>
+        <v>41.10072355711193</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>54.93966700005691</v>
+        <v>39.83247061750857</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>49.82021250450344</v>
+        <v>35.64399333735677</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>43.69215732100776</v>
+        <v>31.09713348419519</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>40.54669231563441</v>
+        <v>28.41580822937094</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>36.32603656294081</v>
+        <v>26.23377085293545</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>35.24440750847005</v>
+        <v>24.75870590791444</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>35.05833221033428</v>
+        <v>24.3766170331294</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>36.37552644126544</v>
+        <v>25.03385651340353</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>37.91088946657828</v>
+        <v>26.5414916231612</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>41.09513507358876</v>
+        <v>27.02952300609039</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>46.75908007707611</v>
+        <v>9.7637121365788</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>52.71355137258262</v>
+        <v>14.57248129075477</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>49.75404360126679</v>
+        <v>51.84894553170169</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>38.91997766776474</v>
+        <v>81.34682791888635</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>36.62314935516316</v>
+        <v>99.07586417766041</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>33.75318898511347</v>
+        <v>95.26711183175858</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>41.1352651030347</v>
+        <v>93.52968324836532</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>46.78009461702231</v>
+        <v>90.36040872657695</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>57.33421688983811</v>
+        <v>82.90586800203631</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>70.86610547770044</v>
+        <v>61.33629436505528</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>75.98877233409968</v>
+        <v>28.24686942960917</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>76.92042216691284</v>
+        <v>5.763760403808174</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>73.38938438637366</v>
+        <v>31.711105051037</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>66.38961151131851</v>
+        <v>41.99304055177493</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>59.9938005072943</v>
+        <v>40.94971982696009</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>53.31422539126781</v>
+        <v>36.08036393078577</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>46.56330397628213</v>
+        <v>31.46730938116832</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>40.78756687954799</v>
+        <v>28.06090862559238</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>37.27939337639029</v>
+        <v>25.59874711077609</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>36.19824571583222</v>
+        <v>24.22361785967955</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>35.74123304681906</v>
+        <v>24.53344358202931</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>36.74552785402163</v>
+        <v>25.02973632294978</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>38.44757792616835</v>
+        <v>26.82266208930907</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>41.51488896248188</v>
+        <v>28.34774711761319</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>47.78984023133718</v>
+        <v>12.68436128430829</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>52.61721286758997</v>
+        <v>17.92779081785294</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>48.276045728056</v>
+        <v>44.47132789784368</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>38.6968609990262</v>
+        <v>69.92092261910811</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>37.66993552806074</v>
+        <v>94.34301627133338</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>38.32864511562358</v>
+        <v>102.5880037674024</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>39.30261529165242</v>
+        <v>104.7901593500661</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>45.95661157591219</v>
+        <v>91.16229048767769</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>56.49468337611947</v>
+        <v>77.19686157826474</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>71.83328801157403</v>
+        <v>46.18125609558001</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>77.6193338452531</v>
+        <v>9.88647873323734</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>77.99333745467698</v>
+        <v>13.72554695315357</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>73.8475096209185</v>
+        <v>32.08322488631979</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>67.67544699872047</v>
+        <v>43.98016358677276</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>60.37560491101446</v>
+        <v>41.83188098302666</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>52.65385414974714</v>
+        <v>36.55051189584609</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>46.44888995790078</v>
+        <v>31.31614897735183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
DRCC constraint tightening implemented
</commit_message>
<xml_diff>
--- a/output/res_trafo/loading_percent.xlsx
+++ b/output/res_trafo/loading_percent.xlsx
@@ -443,7 +443,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="n">
-        <v>60.10334315180501</v>
+        <v>39.70756522553047</v>
       </c>
     </row>
     <row r="3">
@@ -451,7 +451,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>56.58425452548431</v>
+        <v>36.71375351479589</v>
       </c>
     </row>
     <row r="4">
@@ -459,7 +459,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>56.94421150267195</v>
+        <v>36.66199460486842</v>
       </c>
     </row>
     <row r="5">
@@ -467,7 +467,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>58.34103254525552</v>
+        <v>37.5299987015089</v>
       </c>
     </row>
     <row r="6">
@@ -475,7 +475,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>59.37501645809402</v>
+        <v>38.5812510973788</v>
       </c>
     </row>
     <row r="7">
@@ -483,7 +483,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>61.03505327508294</v>
+        <v>40.22749585104386</v>
       </c>
     </row>
     <row r="8">
@@ -491,7 +491,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>65.23688659590925</v>
+        <v>43.1960835690894</v>
       </c>
     </row>
     <row r="9">
@@ -499,7 +499,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>72.04544388204948</v>
+        <v>48.56213034182267</v>
       </c>
     </row>
     <row r="10">
@@ -507,7 +507,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>74.36029136116177</v>
+        <v>50.41620143513571</v>
       </c>
     </row>
     <row r="11">
@@ -515,7 +515,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>66.72257087603609</v>
+        <v>42.80171524673896</v>
       </c>
     </row>
     <row r="12">
@@ -523,7 +523,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>45.2702798753776</v>
+        <v>21.98016798916847</v>
       </c>
     </row>
     <row r="13">
@@ -531,7 +531,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>44.05964152503088</v>
+        <v>22.1802604900965</v>
       </c>
     </row>
     <row r="14">
@@ -539,7 +539,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>45.73344528080362</v>
+        <v>24.2832078961415</v>
       </c>
     </row>
     <row r="15">
@@ -547,7 +547,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>43.92468319318981</v>
+        <v>22.77688586531106</v>
       </c>
     </row>
     <row r="16">
@@ -555,7 +555,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>47.82456692643934</v>
+        <v>26.66903409280029</v>
       </c>
     </row>
     <row r="17">
@@ -563,7 +563,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>62.14064300123883</v>
+        <v>40.20593861197004</v>
       </c>
     </row>
     <row r="18">
@@ -571,7 +571,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>84.41727446235005</v>
+        <v>61.19398225193231</v>
       </c>
     </row>
     <row r="19">
@@ -579,7 +579,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>92.49003387425837</v>
+        <v>68.548383456103</v>
       </c>
     </row>
     <row r="20">
@@ -587,7 +587,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>95.42482762568862</v>
+        <v>71.11191766389766</v>
       </c>
     </row>
     <row r="21">
@@ -595,7 +595,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>93.56183105845648</v>
+        <v>69.42037236716921</v>
       </c>
     </row>
     <row r="22">
@@ -603,7 +603,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>87.72079183557648</v>
+        <v>64.41862480153546</v>
       </c>
     </row>
     <row r="23">
@@ -611,7 +611,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>80.08730544095187</v>
+        <v>57.73788601223821</v>
       </c>
     </row>
     <row r="24">
@@ -619,7 +619,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>74.2848565050659</v>
+        <v>51.90698956703438</v>
       </c>
     </row>
     <row r="25">
@@ -627,7 +627,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>67.52192799910276</v>
+        <v>45.80274229460871</v>
       </c>
     </row>
     <row r="26">
@@ -635,7 +635,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>63.75735189417033</v>
+        <v>41.71069301898779</v>
       </c>
     </row>
     <row r="27">
@@ -643,7 +643,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>61.25091200593624</v>
+        <v>39.20023898363534</v>
       </c>
     </row>
     <row r="28">
@@ -651,7 +651,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>63.37734392460439</v>
+        <v>40.03989335386179</v>
       </c>
     </row>
     <row r="29">
@@ -659,7 +659,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>62.26248322413335</v>
+        <v>39.74443993112113</v>
       </c>
     </row>
     <row r="30">
@@ -667,7 +667,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>63.85422437160122</v>
+        <v>41.10936471497988</v>
       </c>
     </row>
     <row r="31">
@@ -675,7 +675,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>66.26007451673691</v>
+        <v>43.40641907046682</v>
       </c>
     </row>
     <row r="32">
@@ -683,7 +683,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>69.82369844111716</v>
+        <v>46.0204620134806</v>
       </c>
     </row>
     <row r="33">
@@ -691,7 +691,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>74.87719170871519</v>
+        <v>49.60311877151939</v>
       </c>
     </row>
     <row r="34">
@@ -699,7 +699,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>77.51040115361927</v>
+        <v>50.76834291926837</v>
       </c>
     </row>
     <row r="35">
@@ -707,7 +707,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>59.47001378207452</v>
+        <v>33.73695518126696</v>
       </c>
     </row>
     <row r="36">
@@ -715,7 +715,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>31.63448809336388</v>
+        <v>7.486070487360879</v>
       </c>
     </row>
     <row r="37">
@@ -723,7 +723,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>28.94657141413322</v>
+        <v>5.976361548164601</v>
       </c>
     </row>
     <row r="38">
@@ -731,7 +731,7 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>30.04381892076857</v>
+        <v>6.993729666637092</v>
       </c>
     </row>
     <row r="39">
@@ -739,7 +739,7 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>32.17115857826525</v>
+        <v>9.214339427489291</v>
       </c>
     </row>
     <row r="40">
@@ -747,7 +747,7 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>42.16359253256972</v>
+        <v>19.66403328585519</v>
       </c>
     </row>
     <row r="41">
@@ -755,7 +755,7 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>64.20193309846897</v>
+        <v>40.45656745472969</v>
       </c>
     </row>
     <row r="42">
@@ -763,7 +763,7 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>86.25994582890364</v>
+        <v>61.16743276223691</v>
       </c>
     </row>
     <row r="43">
@@ -771,7 +771,7 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>94.76824231234173</v>
+        <v>69.72216146879553</v>
       </c>
     </row>
     <row r="44">
@@ -779,7 +779,7 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>95.00377577078791</v>
+        <v>70.66118570170329</v>
       </c>
     </row>
     <row r="45">
@@ -787,7 +787,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>92.84576042063883</v>
+        <v>69.15938035060162</v>
       </c>
     </row>
     <row r="46">
@@ -795,7 +795,7 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>86.8998046868999</v>
+        <v>64.28249162524909</v>
       </c>
     </row>
     <row r="47">
@@ -803,7 +803,7 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>81.05239488245869</v>
+        <v>58.34421988500732</v>
       </c>
     </row>
     <row r="48">
@@ -811,7 +811,7 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>74.49973685336072</v>
+        <v>51.97796762444506</v>
       </c>
     </row>
     <row r="49">
@@ -819,7 +819,7 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>68.41087730920049</v>
+        <v>46.1553605195133</v>
       </c>
     </row>
     <row r="50">
@@ -827,7 +827,7 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>63.41065558010634</v>
+        <v>41.33662232607034</v>
       </c>
     </row>
     <row r="51">
@@ -835,7 +835,7 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>61.35595993289781</v>
+        <v>39.16045320709952</v>
       </c>
     </row>
     <row r="52">
@@ -843,7 +843,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>60.96162121550308</v>
+        <v>38.8558499446918</v>
       </c>
     </row>
     <row r="53">
@@ -851,7 +851,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>61.19275334487932</v>
+        <v>39.25576685982568</v>
       </c>
     </row>
     <row r="54">
@@ -859,7 +859,7 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>61.41715556727425</v>
+        <v>40.07179501694493</v>
       </c>
     </row>
     <row r="55">
@@ -867,7 +867,7 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>64.38985653439057</v>
+        <v>42.51658503338035</v>
       </c>
     </row>
     <row r="56">
@@ -875,7 +875,7 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>70.34260465533733</v>
+        <v>46.5310819298879</v>
       </c>
     </row>
     <row r="57">
@@ -883,7 +883,7 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>75.83886333616309</v>
+        <v>49.89174247931454</v>
       </c>
     </row>
     <row r="58">
@@ -891,7 +891,7 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>79.39654260602441</v>
+        <v>51.75562941882315</v>
       </c>
     </row>
     <row r="59">
@@ -899,7 +899,7 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>62.21132806685081</v>
+        <v>35.20781052547783</v>
       </c>
     </row>
     <row r="60">
@@ -907,7 +907,7 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>37.0622872013756</v>
+        <v>11.22602316129374</v>
       </c>
     </row>
     <row r="61">
@@ -915,7 +915,7 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>22.05696514450281</v>
+        <v>4.76405825495212</v>
       </c>
     </row>
     <row r="62">
@@ -923,7 +923,7 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>23.93969536512877</v>
+        <v>2.707525466045316</v>
       </c>
     </row>
     <row r="63">
@@ -931,7 +931,7 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>33.1598429438512</v>
+        <v>10.0055351130251</v>
       </c>
     </row>
     <row r="64">
@@ -939,7 +939,7 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>47.0274610147398</v>
+        <v>23.65335470418683</v>
       </c>
     </row>
     <row r="65">
@@ -947,7 +947,7 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>70.01068773439162</v>
+        <v>44.99703781538865</v>
       </c>
     </row>
     <row r="66">
@@ -955,7 +955,7 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>88.79502233380904</v>
+        <v>63.46568711158353</v>
       </c>
     </row>
     <row r="67">
@@ -963,7 +963,7 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>94.68832568498381</v>
+        <v>69.12998154989313</v>
       </c>
     </row>
     <row r="68">
@@ -971,7 +971,7 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>95.57284693565595</v>
+        <v>70.92092678952037</v>
       </c>
     </row>
     <row r="69">
@@ -979,7 +979,7 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>93.18248834400836</v>
+        <v>69.43824802794083</v>
       </c>
     </row>
     <row r="70">
@@ -987,7 +987,7 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>86.88566192454569</v>
+        <v>64.43359375321968</v>
       </c>
     </row>
     <row r="71">
@@ -995,7 +995,7 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>78.18636110642683</v>
+        <v>56.90172343450115</v>
       </c>
     </row>
     <row r="72">
@@ -1003,7 +1003,7 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>71.53946358377526</v>
+        <v>50.37881940481775</v>
       </c>
     </row>
     <row r="73">
@@ -1011,7 +1011,7 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>66.31634213781925</v>
+        <v>44.91806494801488</v>
       </c>
     </row>
     <row r="74">
@@ -1019,7 +1019,7 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>61.31845351448604</v>
+        <v>40.29991638609668</v>
       </c>
     </row>
     <row r="75">
@@ -1027,7 +1027,7 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>58.61978621463696</v>
+        <v>37.85354879538119</v>
       </c>
     </row>
     <row r="76">
@@ -1035,7 +1035,7 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>58.08871339559385</v>
+        <v>37.26864843546885</v>
       </c>
     </row>
     <row r="77">
@@ -1043,7 +1043,7 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>59.23441039822547</v>
+        <v>38.09471336254808</v>
       </c>
     </row>
     <row r="78">
@@ -1051,7 +1051,7 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>60.49907441295291</v>
+        <v>39.34015263724853</v>
       </c>
     </row>
     <row r="79">
@@ -1059,7 +1059,7 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>63.41114763946252</v>
+        <v>41.95942994435474</v>
       </c>
     </row>
     <row r="80">
@@ -1067,7 +1067,7 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>68.41819705915125</v>
+        <v>45.5339922703896</v>
       </c>
     </row>
     <row r="81">
@@ -1075,7 +1075,7 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>73.10404940975334</v>
+        <v>48.68438162796498</v>
       </c>
     </row>
     <row r="82">
@@ -1083,7 +1083,7 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>74.06835133510701</v>
+        <v>49.35117065178061</v>
       </c>
     </row>
     <row r="83">
@@ -1091,7 +1091,7 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>55.55479104349992</v>
+        <v>31.75608746781001</v>
       </c>
     </row>
     <row r="84">
@@ -1099,7 +1099,7 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>34.28503249955978</v>
+        <v>11.40589240943555</v>
       </c>
     </row>
     <row r="85">
@@ -1107,7 +1107,7 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>23.10612724628029</v>
+        <v>2.589960650531623</v>
       </c>
     </row>
     <row r="86">
@@ -1115,7 +1115,7 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>19.67440088988884</v>
+        <v>3.553214114725804</v>
       </c>
     </row>
     <row r="87">
@@ -1123,7 +1123,7 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>27.4874174341605</v>
+        <v>6.820929073306885</v>
       </c>
     </row>
     <row r="88">
@@ -1131,7 +1131,7 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>43.76701139313056</v>
+        <v>23.03069372875257</v>
       </c>
     </row>
     <row r="89">
@@ -1139,7 +1139,7 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>64.38922053295323</v>
+        <v>41.96736665094137</v>
       </c>
     </row>
     <row r="90">
@@ -1147,7 +1147,7 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>82.99981315327911</v>
+        <v>60.02004381277126</v>
       </c>
     </row>
     <row r="91">
@@ -1155,7 +1155,7 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>91.18634490893923</v>
+        <v>67.36568120425713</v>
       </c>
     </row>
     <row r="92">
@@ -1163,7 +1163,7 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>92.7874510026589</v>
+        <v>69.37959933948466</v>
       </c>
     </row>
     <row r="93">
@@ -1171,7 +1171,7 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>91.41119110569061</v>
+        <v>68.32699265393558</v>
       </c>
     </row>
     <row r="94">
@@ -1179,7 +1179,7 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>85.92311213916221</v>
+        <v>63.48606030725556</v>
       </c>
     </row>
     <row r="95">
@@ -1187,7 +1187,7 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>78.76332776700347</v>
+        <v>56.81313840846614</v>
       </c>
     </row>
     <row r="96">
@@ -1195,7 +1195,7 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>71.72906299765891</v>
+        <v>50.42858922152749</v>
       </c>
     </row>
     <row r="97">
@@ -1203,7 +1203,7 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>66.24389142115352</v>
+        <v>44.93926315318741</v>
       </c>
     </row>
     <row r="98">
@@ -1211,7 +1211,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>59.80759924737762</v>
+        <v>39.6157829941471</v>
       </c>
     </row>
     <row r="99">
@@ -1219,7 +1219,7 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>56.79745198998108</v>
+        <v>36.83004614630886</v>
       </c>
     </row>
     <row r="100">
@@ -1227,7 +1227,7 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>55.53861222308305</v>
+        <v>35.60431722197663</v>
       </c>
     </row>
     <row r="101">
@@ -1235,7 +1235,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>55.9963224884395</v>
+        <v>35.88614532603373</v>
       </c>
     </row>
     <row r="102">
@@ -1243,7 +1243,7 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>57.75754030490885</v>
+        <v>37.25675360921436</v>
       </c>
     </row>
     <row r="103">
@@ -1251,7 +1251,7 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>60.50677064766089</v>
+        <v>39.5391231328414</v>
       </c>
     </row>
     <row r="104">
@@ -1259,7 +1259,7 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>64.217054686929</v>
+        <v>42.59296845842366</v>
       </c>
     </row>
     <row r="105">
@@ -1267,7 +1267,7 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>68.548554650654</v>
+        <v>46.05727402400795</v>
       </c>
     </row>
     <row r="106">
@@ -1275,7 +1275,7 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>71.16956891071749</v>
+        <v>48.01430832067471</v>
       </c>
     </row>
     <row r="107">
@@ -1283,7 +1283,7 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>56.65624550835102</v>
+        <v>34.09114126015527</v>
       </c>
     </row>
     <row r="108">
@@ -1291,7 +1291,7 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>38.33212352760133</v>
+        <v>16.5124040099063</v>
       </c>
     </row>
     <row r="109">
@@ -1299,7 +1299,7 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>26.97124478241319</v>
+        <v>6.168202103017451</v>
       </c>
     </row>
     <row r="110">
@@ -1307,7 +1307,7 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>29.27291739760407</v>
+        <v>8.4280964220487</v>
       </c>
     </row>
     <row r="111">
@@ -1315,7 +1315,7 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>34.88474126799919</v>
+        <v>13.85375281391254</v>
       </c>
     </row>
     <row r="112">
@@ -1323,7 +1323,7 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>45.56645047091477</v>
+        <v>24.07144628049327</v>
       </c>
     </row>
     <row r="113">
@@ -1331,7 +1331,7 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>64.29558445655617</v>
+        <v>42.3539635918514</v>
       </c>
     </row>
     <row r="114">
@@ -1339,7 +1339,7 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>83.80082401651127</v>
+        <v>61.12835289820333</v>
       </c>
     </row>
     <row r="115">
@@ -1347,7 +1347,7 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>89.28426838894197</v>
+        <v>66.87676539102986</v>
       </c>
     </row>
     <row r="116">
@@ -1355,7 +1355,7 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>91.48788295194217</v>
+        <v>68.95459150822842</v>
       </c>
     </row>
     <row r="117">
@@ -1363,7 +1363,7 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>85.41524450066375</v>
+        <v>64.37226086101113</v>
       </c>
     </row>
     <row r="118">
@@ -1371,7 +1371,7 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>80.48629821126733</v>
+        <v>59.5904055882508</v>
       </c>
     </row>
     <row r="119">
@@ -1379,7 +1379,7 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>74.79573848078171</v>
+        <v>54.13978052967309</v>
       </c>
     </row>
     <row r="120">
@@ -1387,7 +1387,7 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>70.86673692979889</v>
+        <v>49.77420222948541</v>
       </c>
     </row>
     <row r="121">
@@ -1395,7 +1395,7 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>65.03086133816134</v>
+        <v>44.26369303420297</v>
       </c>
     </row>
     <row r="122">
@@ -1403,7 +1403,7 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>63.29997481132624</v>
+        <v>41.76348166146418</v>
       </c>
     </row>
     <row r="123">
@@ -1411,7 +1411,7 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>58.95635074402394</v>
+        <v>37.93111145836397</v>
       </c>
     </row>
     <row r="124">
@@ -1419,7 +1419,7 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>57.9217424569248</v>
+        <v>36.9646813545253</v>
       </c>
     </row>
     <row r="125">
@@ -1427,7 +1427,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>57.89290385018862</v>
+        <v>36.77416385121867</v>
       </c>
     </row>
     <row r="126">
@@ -1435,7 +1435,7 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>59.71349795216258</v>
+        <v>38.12022869483522</v>
       </c>
     </row>
     <row r="127">
@@ -1443,7 +1443,7 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>61.60063895628564</v>
+        <v>39.51902532987457</v>
       </c>
     </row>
     <row r="128">
@@ -1451,7 +1451,7 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>66.34057971636727</v>
+        <v>42.72679998019077</v>
       </c>
     </row>
     <row r="129">
@@ -1459,7 +1459,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>72.84880228652064</v>
+        <v>47.89268904624001</v>
       </c>
     </row>
     <row r="130">
@@ -1467,7 +1467,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>78.42000093207494</v>
+        <v>52.94467297811963</v>
       </c>
     </row>
     <row r="131">
@@ -1475,7 +1475,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>73.11035769437105</v>
+        <v>47.66992510287945</v>
       </c>
     </row>
     <row r="132">
@@ -1483,7 +1483,7 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>58.88080241439738</v>
+        <v>34.04254135252872</v>
       </c>
     </row>
     <row r="133">
@@ -1491,7 +1491,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>55.50597204428077</v>
+        <v>30.58229885096751</v>
       </c>
     </row>
     <row r="134">
@@ -1499,7 +1499,7 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>51.48896090041131</v>
+        <v>27.13981634829153</v>
       </c>
     </row>
     <row r="135">
@@ -1507,7 +1507,7 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>60.51729517908333</v>
+        <v>35.82989306495785</v>
       </c>
     </row>
     <row r="136">
@@ -1515,7 +1515,7 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>67.73248100661404</v>
+        <v>43.00670044958897</v>
       </c>
     </row>
     <row r="137">
@@ -1523,7 +1523,7 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>80.65466535201134</v>
+        <v>55.15486749062401</v>
       </c>
     </row>
     <row r="138">
@@ -1531,7 +1531,7 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>94.25556281137739</v>
+        <v>68.90422268951339</v>
       </c>
     </row>
     <row r="139">
@@ -1539,7 +1539,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>98.96998522313272</v>
+        <v>73.6397412169313</v>
       </c>
     </row>
     <row r="140">
@@ -1547,7 +1547,7 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>100.6446923494184</v>
+        <v>74.659633168578</v>
       </c>
     </row>
     <row r="141">
@@ -1555,7 +1555,7 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>96.93490197261877</v>
+        <v>71.515689624125</v>
       </c>
     </row>
     <row r="142">
@@ -1563,7 +1563,7 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>89.67921218526349</v>
+        <v>65.1039053710244</v>
       </c>
     </row>
     <row r="143">
@@ -1571,7 +1571,7 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>82.84322752348309</v>
+        <v>59.30545670182228</v>
       </c>
     </row>
     <row r="144">
@@ -1579,7 +1579,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>75.51102658022647</v>
+        <v>53.1469941760658</v>
       </c>
     </row>
     <row r="145">
@@ -1587,7 +1587,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>68.78474394373792</v>
+        <v>47.07941937299629</v>
       </c>
     </row>
     <row r="146">
@@ -1595,7 +1595,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>63.42514608284062</v>
+        <v>41.95702690573184</v>
       </c>
     </row>
     <row r="147">
@@ -1603,7 +1603,7 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>60.99334453702099</v>
+        <v>39.01178410524457</v>
       </c>
     </row>
     <row r="148">
@@ -1611,7 +1611,7 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>59.92476932013013</v>
+        <v>38.03591615112543</v>
       </c>
     </row>
     <row r="149">
@@ -1619,7 +1619,7 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>59.37179764370924</v>
+        <v>37.56770148771789</v>
       </c>
     </row>
     <row r="150">
@@ -1627,7 +1627,7 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>60.54096360135722</v>
+        <v>38.50886058487816</v>
       </c>
     </row>
     <row r="151">
@@ -1635,7 +1635,7 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>62.84431032161615</v>
+        <v>40.15954344023462</v>
       </c>
     </row>
     <row r="152">
@@ -1643,7 +1643,7 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>67.37064514597438</v>
+        <v>43.18695692059477</v>
       </c>
     </row>
     <row r="153">
@@ -1651,7 +1651,7 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>74.76675916621519</v>
+        <v>49.06697845369285</v>
       </c>
     </row>
     <row r="154">
@@ -1659,7 +1659,7 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>79.10818593061144</v>
+        <v>52.91696254504722</v>
       </c>
     </row>
     <row r="155">
@@ -1667,7 +1667,7 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>71.93805184876419</v>
+        <v>46.08915130451822</v>
       </c>
     </row>
     <row r="156">
@@ -1675,7 +1675,7 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>59.83774465149272</v>
+        <v>33.79733743563055</v>
       </c>
     </row>
     <row r="157">
@@ -1683,7 +1683,7 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>56.54102885182799</v>
+        <v>31.65412153540685</v>
       </c>
     </row>
     <row r="158">
@@ -1691,7 +1691,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>56.61903780505192</v>
+        <v>32.09230265200394</v>
       </c>
     </row>
     <row r="159">
@@ -1699,7 +1699,7 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>57.72002535416379</v>
+        <v>33.52805877991772</v>
       </c>
     </row>
     <row r="160">
@@ -1707,7 +1707,7 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>65.60458291130948</v>
+        <v>41.83392451398664</v>
       </c>
     </row>
     <row r="161">
@@ -1715,7 +1715,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>78.12079038767092</v>
+        <v>54.07874491880163</v>
       </c>
     </row>
     <row r="162">
@@ -1723,7 +1723,7 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>95.14252451856372</v>
+        <v>69.71070237378466</v>
       </c>
     </row>
     <row r="163">
@@ -1731,7 +1731,7 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>100.9154546479107</v>
+        <v>75.12169548134821</v>
       </c>
     </row>
     <row r="164">
@@ -1739,7 +1739,7 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>100.8162506978579</v>
+        <v>75.50669905728606</v>
       </c>
     </row>
     <row r="165">
@@ -1747,7 +1747,7 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>95.9271936743655</v>
+        <v>71.6198686202827</v>
       </c>
     </row>
     <row r="166">
@@ -1755,7 +1755,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>89.50891895694649</v>
+        <v>66.01437840484468</v>
       </c>
     </row>
     <row r="167">
@@ -1763,7 +1763,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>82.01814567690425</v>
+        <v>59.40344858669911</v>
       </c>
     </row>
     <row r="168">
@@ -1771,7 +1771,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>74.09006063299012</v>
+        <v>52.40643544772461</v>
       </c>
     </row>
     <row r="169">
@@ -1779,7 +1779,7 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>68.60066236764241</v>
+        <v>46.9536659926598</v>
       </c>
     </row>
   </sheetData>

</xml_diff>